<commit_message>
Implemented basic pivot table refresh.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableDataSourceTypeWorksheet.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableDataSourceTypeWorksheet.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpf\Documents\DELME\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{006CE864-1AA1-4804-9032-24628A9D765E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8805"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId2"/>
+    <pivotCache cacheId="10" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,15 +28,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>Item</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Bike</t>
+  </si>
+  <si>
+    <t>Car</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Skateboard</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Sum of Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -61,132 +95,20 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF999999"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF999999"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="65"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF999999"/>
-      </right>
-      <top style="thin">
-        <color indexed="65"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF999999"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -205,13 +127,29 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Zachary P. Faltersack" refreshedDate="42894.723356944443" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="2">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Michelle C. Lau" refreshedDate="43367.463875578702" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="3" xr:uid="{C3020381-E950-41B0-AE23-9C8F0C4851D2}">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C3:C5" sheet="Sheet1"/>
+    <worksheetSource ref="C3:F6" sheet="Sheet1"/>
   </cacheSource>
-  <cacheFields count="1">
+  <cacheFields count="4">
+    <cacheField name="Number" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3"/>
+    </cacheField>
     <cacheField name="Item" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="2"/>
+      <sharedItems count="3">
+        <s v="Bike"/>
+        <s v="Car"/>
+        <s v="Skateboard"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Color" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Black"/>
+        <s v="Red"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Cost" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="90000"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -223,26 +161,87 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="2">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="3">
   <r>
     <n v="1"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="100"/>
   </r>
   <r>
     <n v="2"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="90000"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="10"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I10:K27" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields count="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12D92A5F-A0D7-4AFB-9E77-C677F9087506}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I10:J16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="4">
     <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
   </pivotFields>
+  <rowFields count="2">
+    <field x="2"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Cost" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -510,119 +509,133 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:K27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C3:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I10" s="1"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="6"/>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="6"/>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="6"/>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="6"/>
-    </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I17" s="4"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="6"/>
-    </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I18" s="4"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="6"/>
-    </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I19" s="4"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="6"/>
-    </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I20" s="4"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-    </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I21" s="4"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="6"/>
-    </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I22" s="4"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="6"/>
-    </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="4"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="6"/>
-    </row>
-    <row r="24" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I24" s="4"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I25" s="4"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="26" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I26" s="4"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="6"/>
-    </row>
-    <row r="27" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I27" s="7"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="9"/>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="4">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="4">
+        <v>90000</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="4">
+        <v>90110</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed refresh pivot table colItems.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/PivotTableDataSourceTypeWorksheet.xlsx
+++ b/EPPlusTest/Workbooks/PivotTableDataSourceTypeWorksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\EPPlus\EPPlusTest\Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{006CE864-1AA1-4804-9032-24628A9D765E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{84240847-B2C8-4DA7-BA9C-BBD84BC76EAA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId2"/>
+    <pivotCache cacheId="4" r:id="rId2"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Michelle C. Lau" refreshedDate="43367.463875578702" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="3" xr:uid="{C3020381-E950-41B0-AE23-9C8F0C4851D2}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Michelle C. Lau" refreshedDate="43384.591185532408" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="3" xr:uid="{C3020381-E950-41B0-AE23-9C8F0C4851D2}">
   <cacheSource type="worksheet">
     <worksheetSource ref="C3:F6" sheet="Sheet1"/>
   </cacheSource>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12D92A5F-A0D7-4AFB-9E77-C677F9087506}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12D92A5F-A0D7-4AFB-9E77-C677F9087506}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I10:J16" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField showAll="0"/>
@@ -513,14 +513,14 @@
   <dimension ref="C3:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="9" max="9" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>